<commit_message>
DB last HW in progress
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestNGFramework.xlsx
+++ b/src/test/resources/testdata/TestNGFramework.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drozz\IdeaProjects\TestNGFramework\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drozz\IdeaProjects\HRMS\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09757CE7-AC01-483C-8A2D-AD9AFD9D9722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC843176-025B-4C4C-A7A9-7EF0C073C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{8764EA60-9503-4497-89AF-DE8C2A1C1078}"/>
   </bookViews>
@@ -88,13 +88,13 @@
     <t>C:\Users\drozz\Pictures\istockphoto-1265423653-170667a.jpg</t>
   </si>
   <si>
-    <t>RG3452346499</t>
-  </si>
-  <si>
-    <t>MC1234399</t>
-  </si>
-  <si>
-    <t>ZZZ1234599</t>
+    <t>RG567345646546</t>
+  </si>
+  <si>
+    <t>MC345346574</t>
+  </si>
+  <si>
+    <t>ZZZ344356546435</t>
   </si>
 </sst>
 </file>

</xml_diff>